<commit_message>
changed zero missingness coding, updated scripts with all percentages
analysis scripts now contain the percentages shown in the manuscript
</commit_message>
<xml_diff>
--- a/data/sim_res.xlsx
+++ b/data/sim_res.xlsx
@@ -8310,7 +8310,7 @@
       </c>
       <c r="P128" t="inlineStr">
         <is>
-          <t>zero missingness</t>
+          <t>not quantified</t>
         </is>
       </c>
       <c r="Q128" t="inlineStr">
@@ -52638,7 +52638,7 @@
       </c>
       <c r="P834" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>not quantified</t>
         </is>
       </c>
       <c r="Q834" t="inlineStr">

</xml_diff>